<commit_message>
retreiving data from excel functionality is done
</commit_message>
<xml_diff>
--- a/extraExpenses.xlsx
+++ b/extraExpenses.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myEco101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95E64A1-86B0-4C6E-AF09-697264DFCF02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420E177B-E4FE-4646-8678-D9DFE62019BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="August" sheetId="1" r:id="rId1"/>
+    <sheet name="AUGUST" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -360,7 +360,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>